<commit_message>
fix: tutorial model Excel files
- fixes #119 by restoring the original gene identifiers in the example models (use YAL054C-like identifiers instead of g1)
</commit_message>
<xml_diff>
--- a/tutorial/smallYeast.xlsx
+++ b/tutorial/smallYeast.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simmarc/Box Sync/3_functions/0_matlab/RAVEN/tutorial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\GitHub\RAVEN\tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{08BA64E1-1B35-4C5A-9706-87D03289F031}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16460"/>
+    <workbookView xWindow="1860" yWindow="435" windowWidth="28800" windowHeight="16455" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RXNS" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="GENES" sheetId="4" r:id="rId4"/>
     <sheet name="MODEL" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1668,237 +1669,6 @@
     <t>TKL1</t>
   </si>
   <si>
-    <t>g1</t>
-  </si>
-  <si>
-    <t>g2</t>
-  </si>
-  <si>
-    <t>g3</t>
-  </si>
-  <si>
-    <t>g4</t>
-  </si>
-  <si>
-    <t>g5</t>
-  </si>
-  <si>
-    <t>g6</t>
-  </si>
-  <si>
-    <t>g7</t>
-  </si>
-  <si>
-    <t>g8</t>
-  </si>
-  <si>
-    <t>g9</t>
-  </si>
-  <si>
-    <t>g10</t>
-  </si>
-  <si>
-    <t>g11</t>
-  </si>
-  <si>
-    <t>g12</t>
-  </si>
-  <si>
-    <t>g13</t>
-  </si>
-  <si>
-    <t>g14</t>
-  </si>
-  <si>
-    <t>g15</t>
-  </si>
-  <si>
-    <t>g16</t>
-  </si>
-  <si>
-    <t>g17</t>
-  </si>
-  <si>
-    <t>g18</t>
-  </si>
-  <si>
-    <t>g19</t>
-  </si>
-  <si>
-    <t>g20</t>
-  </si>
-  <si>
-    <t>g21</t>
-  </si>
-  <si>
-    <t>g22</t>
-  </si>
-  <si>
-    <t>g23</t>
-  </si>
-  <si>
-    <t>g24</t>
-  </si>
-  <si>
-    <t>g25</t>
-  </si>
-  <si>
-    <t>g26</t>
-  </si>
-  <si>
-    <t>g27</t>
-  </si>
-  <si>
-    <t>g28</t>
-  </si>
-  <si>
-    <t>g29</t>
-  </si>
-  <si>
-    <t>g30</t>
-  </si>
-  <si>
-    <t>g31</t>
-  </si>
-  <si>
-    <t>g32</t>
-  </si>
-  <si>
-    <t>g33</t>
-  </si>
-  <si>
-    <t>g34</t>
-  </si>
-  <si>
-    <t>g35</t>
-  </si>
-  <si>
-    <t>g36</t>
-  </si>
-  <si>
-    <t>g37</t>
-  </si>
-  <si>
-    <t>g38</t>
-  </si>
-  <si>
-    <t>g39</t>
-  </si>
-  <si>
-    <t>g40</t>
-  </si>
-  <si>
-    <t>g41</t>
-  </si>
-  <si>
-    <t>g42</t>
-  </si>
-  <si>
-    <t>g43</t>
-  </si>
-  <si>
-    <t>g44</t>
-  </si>
-  <si>
-    <t>g45</t>
-  </si>
-  <si>
-    <t>g46</t>
-  </si>
-  <si>
-    <t>g47</t>
-  </si>
-  <si>
-    <t>g48</t>
-  </si>
-  <si>
-    <t>g49</t>
-  </si>
-  <si>
-    <t>g50</t>
-  </si>
-  <si>
-    <t>g51</t>
-  </si>
-  <si>
-    <t>g52</t>
-  </si>
-  <si>
-    <t>g53</t>
-  </si>
-  <si>
-    <t>g54</t>
-  </si>
-  <si>
-    <t>g55</t>
-  </si>
-  <si>
-    <t>g56</t>
-  </si>
-  <si>
-    <t>g57</t>
-  </si>
-  <si>
-    <t>g58</t>
-  </si>
-  <si>
-    <t>g59</t>
-  </si>
-  <si>
-    <t>g60</t>
-  </si>
-  <si>
-    <t>g61</t>
-  </si>
-  <si>
-    <t>(g14 or g16 or g5)</t>
-  </si>
-  <si>
-    <t>(g20 or g47)</t>
-  </si>
-  <si>
-    <t>(g30 or g32 or g19)</t>
-  </si>
-  <si>
-    <t>(g38 or g8 or g52)</t>
-  </si>
-  <si>
-    <t>(g23 or g26)</t>
-  </si>
-  <si>
-    <t>(g51 or g7 or g25 or g22)</t>
-  </si>
-  <si>
-    <t>(g24 or g27)</t>
-  </si>
-  <si>
-    <t>(g2 or g61)</t>
-  </si>
-  <si>
-    <t>(g9 or g53)</t>
-  </si>
-  <si>
-    <t>(g28 or g12)</t>
-  </si>
-  <si>
-    <t>(g18 or g41 or g40)</t>
-  </si>
-  <si>
-    <t>(g17 or g48 or g54)</t>
-  </si>
-  <si>
-    <t>(g1 or g42)</t>
-  </si>
-  <si>
-    <t>(g15 or g4)</t>
-  </si>
-  <si>
-    <t>(g50 or g60)</t>
-  </si>
-  <si>
-    <t>(g21 or g56)</t>
-  </si>
-  <si>
     <t>kegg.genes/sce:YAL054C;sgd/S000000050;uniprot/Q01574</t>
   </si>
   <si>
@@ -2080,12 +1850,243 @@
   </si>
   <si>
     <t>kegg.genes/sce:YPR074C;sgd/S000006278;uniprot/P23254</t>
+  </si>
+  <si>
+    <t>YFR053C or YGL253W or YCL040W</t>
+  </si>
+  <si>
+    <t>YBR196C</t>
+  </si>
+  <si>
+    <t>YGR240C or YMR205C</t>
+  </si>
+  <si>
+    <t>YLR377C</t>
+  </si>
+  <si>
+    <t>YKL060C</t>
+  </si>
+  <si>
+    <t>YDR050C</t>
+  </si>
+  <si>
+    <t>YJL052W or YJR009C or YGR192C</t>
+  </si>
+  <si>
+    <t>YCR012W</t>
+  </si>
+  <si>
+    <t>YKL152C or YDL021W or YOL056W</t>
+  </si>
+  <si>
+    <t>YGR254W or YHR174W</t>
+  </si>
+  <si>
+    <t>YOR347C</t>
+  </si>
+  <si>
+    <t>YNL241C</t>
+  </si>
+  <si>
+    <t>YNR034W or YCR073W-A or YHR163W or YGR248W</t>
+  </si>
+  <si>
+    <t>YGR256W or YHR183W</t>
+  </si>
+  <si>
+    <t>YOR095C</t>
+  </si>
+  <si>
+    <t>YJL121C</t>
+  </si>
+  <si>
+    <t>YBR117C or YPR074C</t>
+  </si>
+  <si>
+    <t>YLR354C</t>
+  </si>
+  <si>
+    <t>YDL022W or YOL059W</t>
+  </si>
+  <si>
+    <t>YIL053W or YER062C</t>
+  </si>
+  <si>
+    <t>YGR087C or YLR134W or YLR044C</t>
+  </si>
+  <si>
+    <t>YGL256W or YMR303C or YOL086C</t>
+  </si>
+  <si>
+    <t>YPL061W</t>
+  </si>
+  <si>
+    <t>YAL054C or YLR153C</t>
+  </si>
+  <si>
+    <t>YER178W</t>
+  </si>
+  <si>
+    <t>YGL062W or YBR218C</t>
+  </si>
+  <si>
+    <t>YNR001C or YPR001W</t>
+  </si>
+  <si>
+    <t>YLR304C</t>
+  </si>
+  <si>
+    <t>YDL066W</t>
+  </si>
+  <si>
+    <t>YIL125W</t>
+  </si>
+  <si>
+    <t>YGR244C or YOR142W</t>
+  </si>
+  <si>
+    <t>YKL141W</t>
+  </si>
+  <si>
+    <t>YJR051W</t>
+  </si>
+  <si>
+    <t>YPL262W</t>
+  </si>
+  <si>
+    <t>YKL085W</t>
+  </si>
+  <si>
+    <t>YKL029C</t>
+  </si>
+  <si>
+    <t>YKR097W</t>
+  </si>
+  <si>
+    <t>YML042W</t>
+  </si>
+  <si>
+    <t>YAL054C</t>
+  </si>
+  <si>
+    <t>YBR117C</t>
+  </si>
+  <si>
+    <t>YBR218C</t>
+  </si>
+  <si>
+    <t>YCL040W</t>
+  </si>
+  <si>
+    <t>YCR073W-A</t>
+  </si>
+  <si>
+    <t>YDL021W</t>
+  </si>
+  <si>
+    <t>YDL022W</t>
+  </si>
+  <si>
+    <t>YER062C</t>
+  </si>
+  <si>
+    <t>YFR053C</t>
+  </si>
+  <si>
+    <t>YGL062W</t>
+  </si>
+  <si>
+    <t>YGL253W</t>
+  </si>
+  <si>
+    <t>YGL256W</t>
+  </si>
+  <si>
+    <t>YGR087C</t>
+  </si>
+  <si>
+    <t>YGR192C</t>
+  </si>
+  <si>
+    <t>YGR240C</t>
+  </si>
+  <si>
+    <t>YGR244C</t>
+  </si>
+  <si>
+    <t>YGR248W</t>
+  </si>
+  <si>
+    <t>YGR254W</t>
+  </si>
+  <si>
+    <t>YGR256W</t>
+  </si>
+  <si>
+    <t>YHR163W</t>
+  </si>
+  <si>
+    <t>YHR174W</t>
+  </si>
+  <si>
+    <t>YHR183W</t>
+  </si>
+  <si>
+    <t>YIL053W</t>
+  </si>
+  <si>
+    <t>YJL052W</t>
+  </si>
+  <si>
+    <t>YJR009C</t>
+  </si>
+  <si>
+    <t>YKL152C</t>
+  </si>
+  <si>
+    <t>YLR044C</t>
+  </si>
+  <si>
+    <t>YLR134W</t>
+  </si>
+  <si>
+    <t>YLR153C</t>
+  </si>
+  <si>
+    <t>YMR205C</t>
+  </si>
+  <si>
+    <t>YMR303C</t>
+  </si>
+  <si>
+    <t>YNR001C</t>
+  </si>
+  <si>
+    <t>YNR034W</t>
+  </si>
+  <si>
+    <t>YOL056W</t>
+  </si>
+  <si>
+    <t>YOL059W</t>
+  </si>
+  <si>
+    <t>YOL086C</t>
+  </si>
+  <si>
+    <t>YOR142W</t>
+  </si>
+  <si>
+    <t>YPR001W</t>
+  </si>
+  <si>
+    <t>YPR074C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2098,26 +2099,31 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2148,7 +2154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2156,7 +2162,6 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2172,6 +2177,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2439,32 +2447,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14:F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="61.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" customWidth="1"/>
-    <col min="7" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" customWidth="1"/>
-    <col min="14" max="15" width="30.6640625" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="12" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2514,19 +2522,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+    <row r="2" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>489</v>
       </c>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
@@ -2540,7 +2548,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2557,7 +2565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2571,7 +2579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
@@ -2585,7 +2593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
@@ -2599,7 +2607,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
@@ -2616,7 +2624,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2633,7 +2641,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
@@ -2650,19 +2658,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C12" s="13"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>41</v>
       </c>
@@ -2679,7 +2687,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>45</v>
       </c>
@@ -2690,13 +2698,13 @@
         <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>547</v>
+        <v>607</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>48</v>
       </c>
@@ -2707,13 +2715,13 @@
         <v>50</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>51</v>
       </c>
@@ -2724,13 +2732,13 @@
         <v>53</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>54</v>
       </c>
@@ -2741,13 +2749,13 @@
         <v>56</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>579</v>
+        <v>610</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>57</v>
       </c>
@@ -2758,13 +2766,13 @@
         <v>59</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>555</v>
+        <v>611</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>60</v>
       </c>
@@ -2775,13 +2783,13 @@
         <v>62</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>63</v>
       </c>
@@ -2792,13 +2800,13 @@
         <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>550</v>
+        <v>613</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>66</v>
       </c>
@@ -2809,13 +2817,13 @@
         <v>68</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>69</v>
       </c>
@@ -2826,13 +2834,13 @@
         <v>71</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>72</v>
       </c>
@@ -2843,13 +2851,13 @@
         <v>74</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>601</v>
+        <v>616</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>75</v>
       </c>
@@ -2860,13 +2868,13 @@
         <v>77</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>593</v>
+        <v>617</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>78</v>
       </c>
@@ -2877,13 +2885,13 @@
         <v>80</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>611</v>
+        <v>618</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>81</v>
       </c>
@@ -2894,13 +2902,13 @@
         <v>83</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>612</v>
+        <v>619</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>84</v>
       </c>
@@ -2911,13 +2919,13 @@
         <v>86</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>599</v>
+        <v>620</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>87</v>
       </c>
@@ -2928,13 +2936,13 @@
         <v>89</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>575</v>
+        <v>621</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>90</v>
       </c>
@@ -2945,13 +2953,13 @@
         <v>92</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>93</v>
       </c>
@@ -2962,13 +2970,13 @@
         <v>95</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>588</v>
+        <v>623</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>96</v>
       </c>
@@ -2979,13 +2987,13 @@
         <v>97</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>98</v>
       </c>
@@ -2996,13 +3004,13 @@
         <v>100</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>614</v>
+        <v>624</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>101</v>
       </c>
@@ -3013,13 +3021,13 @@
         <v>103</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>104</v>
       </c>
@@ -3030,13 +3038,13 @@
         <v>106</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>616</v>
+        <v>626</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>107</v>
       </c>
@@ -3047,13 +3055,13 @@
         <v>109</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>617</v>
+        <v>627</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>110</v>
       </c>
@@ -3064,13 +3072,13 @@
         <v>112</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>602</v>
+        <v>628</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>113</v>
       </c>
@@ -3081,13 +3089,13 @@
         <v>115</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>618</v>
+        <v>629</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>116</v>
       </c>
@@ -3098,13 +3106,13 @@
         <v>118</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>557</v>
+        <v>630</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>120</v>
       </c>
@@ -3115,13 +3123,13 @@
         <v>122</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>619</v>
+        <v>631</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>123</v>
       </c>
@@ -3132,13 +3140,13 @@
         <v>125</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>620</v>
+        <v>632</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>126</v>
       </c>
@@ -3149,13 +3157,13 @@
         <v>128</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>587</v>
+        <v>633</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>129</v>
       </c>
@@ -3166,13 +3174,13 @@
         <v>131</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>554</v>
+        <v>634</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>132</v>
       </c>
@@ -3183,13 +3191,13 @@
         <v>134</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>573</v>
+        <v>635</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>135</v>
       </c>
@@ -3200,13 +3208,13 @@
         <v>137</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>621</v>
+        <v>636</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>138</v>
       </c>
@@ -3217,13 +3225,13 @@
         <v>140</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>581</v>
+        <v>637</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>141</v>
       </c>
@@ -3234,13 +3242,13 @@
         <v>143</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>577</v>
+        <v>638</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>144</v>
       </c>
@@ -3251,13 +3259,13 @@
         <v>146</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>603</v>
+        <v>639</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>147</v>
       </c>
@@ -3268,13 +3276,13 @@
         <v>149</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>580</v>
+        <v>640</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>150</v>
       </c>
@@ -3285,13 +3293,13 @@
         <v>152</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>578</v>
+        <v>641</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>153</v>
       </c>
@@ -3302,13 +3310,13 @@
         <v>155</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>583</v>
+        <v>642</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>156</v>
       </c>
@@ -3319,13 +3327,13 @@
         <v>158</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>590</v>
+        <v>643</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>159</v>
       </c>
@@ -3339,19 +3347,19 @@
         <v>119</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C54" s="13"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" s="11" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="12"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="10" t="s">
         <v>491</v>
       </c>
-      <c r="C55" s="13"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C55" s="12"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>162</v>
       </c>
@@ -3365,7 +3373,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>165</v>
       </c>
@@ -3379,7 +3387,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>168</v>
       </c>
@@ -3393,7 +3401,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>171</v>
       </c>
@@ -3407,7 +3415,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>174</v>
       </c>
@@ -3427,7 +3435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3435,18 +3443,18 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="7" width="30.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3478,7 +3486,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>181</v>
       </c>
@@ -3501,7 +3509,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>187</v>
       </c>
@@ -3524,7 +3532,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>193</v>
       </c>
@@ -3547,7 +3555,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>199</v>
       </c>
@@ -3570,7 +3578,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>204</v>
       </c>
@@ -3593,7 +3601,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>210</v>
       </c>
@@ -3616,7 +3624,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>216</v>
       </c>
@@ -3639,7 +3647,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>222</v>
       </c>
@@ -3662,7 +3670,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>228</v>
       </c>
@@ -3685,7 +3693,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>234</v>
       </c>
@@ -3711,7 +3719,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>236</v>
       </c>
@@ -3734,7 +3742,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>242</v>
       </c>
@@ -3757,7 +3765,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>244</v>
       </c>
@@ -3780,7 +3788,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>250</v>
       </c>
@@ -3803,7 +3811,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>256</v>
       </c>
@@ -3829,7 +3837,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>258</v>
       </c>
@@ -3852,7 +3860,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>264</v>
       </c>
@@ -3875,7 +3883,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>270</v>
       </c>
@@ -3898,7 +3906,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>276</v>
       </c>
@@ -3921,7 +3929,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>281</v>
       </c>
@@ -3935,7 +3943,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>284</v>
       </c>
@@ -3952,7 +3960,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>286</v>
       </c>
@@ -3975,7 +3983,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>292</v>
       </c>
@@ -3998,7 +4006,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>297</v>
       </c>
@@ -4021,7 +4029,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>299</v>
       </c>
@@ -4047,7 +4055,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>301</v>
       </c>
@@ -4070,7 +4078,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>307</v>
       </c>
@@ -4093,7 +4101,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>309</v>
       </c>
@@ -4116,7 +4124,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>315</v>
       </c>
@@ -4139,7 +4147,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>321</v>
       </c>
@@ -4162,7 +4170,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>327</v>
       </c>
@@ -4185,7 +4193,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>332</v>
       </c>
@@ -4208,7 +4216,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>337</v>
       </c>
@@ -4231,7 +4239,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>343</v>
       </c>
@@ -4257,7 +4265,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>345</v>
       </c>
@@ -4280,7 +4288,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>351</v>
       </c>
@@ -4303,7 +4311,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>357</v>
       </c>
@@ -4326,7 +4334,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>363</v>
       </c>
@@ -4349,7 +4357,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>369</v>
       </c>
@@ -4375,7 +4383,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
         <v>371</v>
       </c>
@@ -4395,7 +4403,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>376</v>
       </c>
@@ -4418,7 +4426,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>381</v>
       </c>
@@ -4441,7 +4449,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>386</v>
       </c>
@@ -4464,7 +4472,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>392</v>
       </c>
@@ -4487,7 +4495,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>394</v>
       </c>
@@ -4510,7 +4518,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>400</v>
       </c>
@@ -4533,7 +4541,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>402</v>
       </c>
@@ -4556,7 +4564,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>408</v>
       </c>
@@ -4579,7 +4587,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>410</v>
       </c>
@@ -4602,7 +4610,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>416</v>
       </c>
@@ -4625,7 +4633,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>418</v>
       </c>
@@ -4648,7 +4656,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>423</v>
       </c>
@@ -4674,7 +4682,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>425</v>
       </c>
@@ -4697,7 +4705,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>431</v>
       </c>
@@ -4720,7 +4728,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>437</v>
       </c>
@@ -4743,7 +4751,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>443</v>
       </c>
@@ -4766,7 +4774,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
         <v>449</v>
       </c>
@@ -4789,7 +4797,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>455</v>
       </c>
@@ -4812,7 +4820,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>461</v>
       </c>
@@ -4841,7 +4849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4849,16 +4857,16 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4875,7 +4883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>44</v>
       </c>
@@ -4883,7 +4891,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>119</v>
       </c>
@@ -4891,7 +4899,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4905,46 +4913,46 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>644</v>
+      </c>
+      <c r="C2" t="s">
         <v>545</v>
-      </c>
-      <c r="C2" t="s">
-        <v>622</v>
       </c>
       <c r="D2" t="s">
         <v>492</v>
@@ -4953,12 +4961,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>645</v>
+      </c>
+      <c r="C3" t="s">
         <v>546</v>
-      </c>
-      <c r="C3" t="s">
-        <v>623</v>
       </c>
       <c r="D3" t="s">
         <v>493</v>
@@ -4967,12 +4975,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>607</v>
+      </c>
+      <c r="C4" t="s">
         <v>547</v>
-      </c>
-      <c r="C4" t="s">
-        <v>624</v>
       </c>
       <c r="D4" t="s">
         <v>494</v>
@@ -4981,12 +4989,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>646</v>
+      </c>
+      <c r="C5" t="s">
         <v>548</v>
-      </c>
-      <c r="C5" t="s">
-        <v>625</v>
       </c>
       <c r="D5" t="s">
         <v>495</v>
@@ -4995,12 +5003,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>647</v>
+      </c>
+      <c r="C6" t="s">
         <v>549</v>
-      </c>
-      <c r="C6" t="s">
-        <v>626</v>
       </c>
       <c r="D6" t="s">
         <v>496</v>
@@ -5009,12 +5017,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C7" t="s">
         <v>550</v>
-      </c>
-      <c r="C7" t="s">
-        <v>627</v>
       </c>
       <c r="D7" t="s">
         <v>497</v>
@@ -5023,12 +5031,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>648</v>
+      </c>
+      <c r="C8" t="s">
         <v>551</v>
-      </c>
-      <c r="C8" t="s">
-        <v>628</v>
       </c>
       <c r="D8" t="s">
         <v>498</v>
@@ -5037,12 +5045,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>649</v>
+      </c>
+      <c r="C9" t="s">
         <v>552</v>
-      </c>
-      <c r="C9" t="s">
-        <v>629</v>
       </c>
       <c r="D9" t="s">
         <v>499</v>
@@ -5051,12 +5059,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>650</v>
+      </c>
+      <c r="C10" t="s">
         <v>553</v>
-      </c>
-      <c r="C10" t="s">
-        <v>630</v>
       </c>
       <c r="D10" t="s">
         <v>500</v>
@@ -5065,12 +5073,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>634</v>
+      </c>
+      <c r="C11" t="s">
         <v>554</v>
-      </c>
-      <c r="C11" t="s">
-        <v>631</v>
       </c>
       <c r="D11" t="s">
         <v>129</v>
@@ -5079,12 +5087,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>611</v>
+      </c>
+      <c r="C12" t="s">
         <v>555</v>
-      </c>
-      <c r="C12" t="s">
-        <v>632</v>
       </c>
       <c r="D12" t="s">
         <v>501</v>
@@ -5093,12 +5101,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>651</v>
+      </c>
+      <c r="C13" t="s">
         <v>556</v>
-      </c>
-      <c r="C13" t="s">
-        <v>633</v>
       </c>
       <c r="D13" t="s">
         <v>502</v>
@@ -5107,12 +5115,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>630</v>
+      </c>
+      <c r="C14" t="s">
         <v>557</v>
-      </c>
-      <c r="C14" t="s">
-        <v>634</v>
       </c>
       <c r="D14" t="s">
         <v>503</v>
@@ -5121,12 +5129,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>652</v>
+      </c>
+      <c r="C15" t="s">
         <v>558</v>
-      </c>
-      <c r="C15" t="s">
-        <v>635</v>
       </c>
       <c r="D15" t="s">
         <v>504</v>
@@ -5135,12 +5143,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>653</v>
+      </c>
+      <c r="C16" t="s">
         <v>559</v>
-      </c>
-      <c r="C16" t="s">
-        <v>636</v>
       </c>
       <c r="D16" t="s">
         <v>505</v>
@@ -5149,12 +5157,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>654</v>
+      </c>
+      <c r="C17" t="s">
         <v>560</v>
-      </c>
-      <c r="C17" t="s">
-        <v>637</v>
       </c>
       <c r="D17" t="s">
         <v>506</v>
@@ -5163,12 +5171,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="7" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>655</v>
+      </c>
+      <c r="C18" t="s">
         <v>561</v>
-      </c>
-      <c r="C18" t="s">
-        <v>638</v>
       </c>
       <c r="D18" t="s">
         <v>507</v>
@@ -5177,12 +5185,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>656</v>
+      </c>
+      <c r="C19" t="s">
         <v>562</v>
-      </c>
-      <c r="C19" t="s">
-        <v>639</v>
       </c>
       <c r="D19" t="s">
         <v>508</v>
@@ -5191,12 +5199,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>657</v>
+      </c>
+      <c r="C20" t="s">
         <v>563</v>
-      </c>
-      <c r="C20" t="s">
-        <v>640</v>
       </c>
       <c r="D20" t="s">
         <v>509</v>
@@ -5205,12 +5213,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>658</v>
+      </c>
+      <c r="C21" t="s">
         <v>564</v>
-      </c>
-      <c r="C21" t="s">
-        <v>641</v>
       </c>
       <c r="D21" t="s">
         <v>510</v>
@@ -5219,12 +5227,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="7" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>659</v>
+      </c>
+      <c r="C22" t="s">
         <v>565</v>
-      </c>
-      <c r="C22" t="s">
-        <v>642</v>
       </c>
       <c r="D22" t="s">
         <v>511</v>
@@ -5233,12 +5241,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="7" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>660</v>
+      </c>
+      <c r="C23" t="s">
         <v>566</v>
-      </c>
-      <c r="C23" t="s">
-        <v>643</v>
       </c>
       <c r="D23" t="s">
         <v>512</v>
@@ -5247,12 +5255,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="7" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>661</v>
+      </c>
+      <c r="C24" t="s">
         <v>567</v>
-      </c>
-      <c r="C24" t="s">
-        <v>644</v>
       </c>
       <c r="D24" t="s">
         <v>513</v>
@@ -5261,12 +5269,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="7" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>662</v>
+      </c>
+      <c r="C25" t="s">
         <v>568</v>
-      </c>
-      <c r="C25" t="s">
-        <v>645</v>
       </c>
       <c r="D25" t="s">
         <v>514</v>
@@ -5275,12 +5283,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="7" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>663</v>
+      </c>
+      <c r="C26" t="s">
         <v>569</v>
-      </c>
-      <c r="C26" t="s">
-        <v>646</v>
       </c>
       <c r="D26" t="s">
         <v>515</v>
@@ -5289,12 +5297,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="7" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>664</v>
+      </c>
+      <c r="C27" t="s">
         <v>570</v>
-      </c>
-      <c r="C27" t="s">
-        <v>647</v>
       </c>
       <c r="D27" t="s">
         <v>516</v>
@@ -5303,12 +5311,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="7" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>665</v>
+      </c>
+      <c r="C28" t="s">
         <v>571</v>
-      </c>
-      <c r="C28" t="s">
-        <v>648</v>
       </c>
       <c r="D28" t="s">
         <v>517</v>
@@ -5317,12 +5325,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="7" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>666</v>
+      </c>
+      <c r="C29" t="s">
         <v>572</v>
-      </c>
-      <c r="C29" t="s">
-        <v>649</v>
       </c>
       <c r="D29" t="s">
         <v>518</v>
@@ -5331,12 +5339,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="7" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>635</v>
+      </c>
+      <c r="C30" t="s">
         <v>573</v>
-      </c>
-      <c r="C30" t="s">
-        <v>650</v>
       </c>
       <c r="D30" t="s">
         <v>519</v>
@@ -5345,12 +5353,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="7" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>667</v>
+      </c>
+      <c r="C31" t="s">
         <v>574</v>
-      </c>
-      <c r="C31" t="s">
-        <v>651</v>
       </c>
       <c r="D31" t="s">
         <v>520</v>
@@ -5359,12 +5367,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="7" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>621</v>
+      </c>
+      <c r="C32" t="s">
         <v>575</v>
-      </c>
-      <c r="C32" t="s">
-        <v>652</v>
       </c>
       <c r="D32" t="s">
         <v>521</v>
@@ -5373,12 +5381,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="7" t="s">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>668</v>
+      </c>
+      <c r="C33" t="s">
         <v>576</v>
-      </c>
-      <c r="C33" t="s">
-        <v>653</v>
       </c>
       <c r="D33" t="s">
         <v>522</v>
@@ -5387,12 +5395,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="7" t="s">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>638</v>
+      </c>
+      <c r="C34" t="s">
         <v>577</v>
-      </c>
-      <c r="C34" t="s">
-        <v>654</v>
       </c>
       <c r="D34" t="s">
         <v>523</v>
@@ -5401,12 +5409,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="7" t="s">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>641</v>
+      </c>
+      <c r="C35" t="s">
         <v>578</v>
-      </c>
-      <c r="C35" t="s">
-        <v>655</v>
       </c>
       <c r="D35" t="s">
         <v>150</v>
@@ -5415,12 +5423,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="7" t="s">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>610</v>
+      </c>
+      <c r="C36" t="s">
         <v>579</v>
-      </c>
-      <c r="C36" t="s">
-        <v>656</v>
       </c>
       <c r="D36" t="s">
         <v>524</v>
@@ -5429,12 +5437,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="7" t="s">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>640</v>
+      </c>
+      <c r="C37" t="s">
         <v>580</v>
-      </c>
-      <c r="C37" t="s">
-        <v>657</v>
       </c>
       <c r="D37" t="s">
         <v>147</v>
@@ -5443,12 +5451,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="7" t="s">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>637</v>
+      </c>
+      <c r="C38" t="s">
         <v>581</v>
-      </c>
-      <c r="C38" t="s">
-        <v>658</v>
       </c>
       <c r="D38" t="s">
         <v>525</v>
@@ -5457,12 +5465,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="7" t="s">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>669</v>
+      </c>
+      <c r="C39" t="s">
         <v>582</v>
-      </c>
-      <c r="C39" t="s">
-        <v>659</v>
       </c>
       <c r="D39" t="s">
         <v>526</v>
@@ -5471,12 +5479,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="7" t="s">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>642</v>
+      </c>
+      <c r="C40" t="s">
         <v>583</v>
-      </c>
-      <c r="C40" t="s">
-        <v>660</v>
       </c>
       <c r="D40" t="s">
         <v>527</v>
@@ -5485,12 +5493,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="7" t="s">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>670</v>
+      </c>
+      <c r="C41" t="s">
         <v>584</v>
-      </c>
-      <c r="C41" t="s">
-        <v>661</v>
       </c>
       <c r="D41" t="s">
         <v>528</v>
@@ -5499,12 +5507,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="7" t="s">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>671</v>
+      </c>
+      <c r="C42" t="s">
         <v>585</v>
-      </c>
-      <c r="C42" t="s">
-        <v>662</v>
       </c>
       <c r="D42" t="s">
         <v>529</v>
@@ -5513,12 +5521,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="7" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>672</v>
+      </c>
+      <c r="C43" t="s">
         <v>586</v>
-      </c>
-      <c r="C43" t="s">
-        <v>663</v>
       </c>
       <c r="D43" t="s">
         <v>530</v>
@@ -5527,12 +5535,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="7" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>633</v>
+      </c>
+      <c r="C44" t="s">
         <v>587</v>
-      </c>
-      <c r="C44" t="s">
-        <v>664</v>
       </c>
       <c r="D44" t="s">
         <v>531</v>
@@ -5541,12 +5549,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="7" t="s">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>623</v>
+      </c>
+      <c r="C45" t="s">
         <v>588</v>
-      </c>
-      <c r="C45" t="s">
-        <v>665</v>
       </c>
       <c r="D45" t="s">
         <v>93</v>
@@ -5555,12 +5563,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="7" t="s">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>609</v>
+      </c>
+      <c r="C46" t="s">
         <v>589</v>
-      </c>
-      <c r="C46" t="s">
-        <v>666</v>
       </c>
       <c r="D46" t="s">
         <v>532</v>
@@ -5569,12 +5577,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B47" s="7" t="s">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>643</v>
+      </c>
+      <c r="C47" t="s">
         <v>590</v>
-      </c>
-      <c r="C47" t="s">
-        <v>667</v>
       </c>
       <c r="D47" t="s">
         <v>156</v>
@@ -5583,12 +5591,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="7" t="s">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>673</v>
+      </c>
+      <c r="C48" t="s">
         <v>591</v>
-      </c>
-      <c r="C48" t="s">
-        <v>668</v>
       </c>
       <c r="D48" t="s">
         <v>533</v>
@@ -5597,12 +5605,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" s="7" t="s">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>674</v>
+      </c>
+      <c r="C49" t="s">
         <v>592</v>
-      </c>
-      <c r="C49" t="s">
-        <v>669</v>
       </c>
       <c r="D49" t="s">
         <v>534</v>
@@ -5611,12 +5619,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="7" t="s">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>617</v>
+      </c>
+      <c r="C50" t="s">
         <v>593</v>
-      </c>
-      <c r="C50" t="s">
-        <v>670</v>
       </c>
       <c r="D50" t="s">
         <v>535</v>
@@ -5625,12 +5633,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="7" t="s">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>675</v>
+      </c>
+      <c r="C51" t="s">
         <v>594</v>
-      </c>
-      <c r="C51" t="s">
-        <v>671</v>
       </c>
       <c r="D51" t="s">
         <v>536</v>
@@ -5639,12 +5647,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B52" s="7" t="s">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>676</v>
+      </c>
+      <c r="C52" t="s">
         <v>595</v>
-      </c>
-      <c r="C52" t="s">
-        <v>672</v>
       </c>
       <c r="D52" t="s">
         <v>537</v>
@@ -5653,12 +5661,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B53" s="7" t="s">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>677</v>
+      </c>
+      <c r="C53" t="s">
         <v>596</v>
-      </c>
-      <c r="C53" t="s">
-        <v>673</v>
       </c>
       <c r="D53" t="s">
         <v>538</v>
@@ -5667,12 +5675,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B54" s="7" t="s">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>678</v>
+      </c>
+      <c r="C54" t="s">
         <v>597</v>
-      </c>
-      <c r="C54" t="s">
-        <v>674</v>
       </c>
       <c r="D54" t="s">
         <v>539</v>
@@ -5681,12 +5689,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B55" s="7" t="s">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>679</v>
+      </c>
+      <c r="C55" t="s">
         <v>598</v>
-      </c>
-      <c r="C55" t="s">
-        <v>675</v>
       </c>
       <c r="D55" t="s">
         <v>107</v>
@@ -5695,12 +5703,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B56" s="7" t="s">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>620</v>
+      </c>
+      <c r="C56" t="s">
         <v>599</v>
-      </c>
-      <c r="C56" t="s">
-        <v>676</v>
       </c>
       <c r="D56" t="s">
         <v>540</v>
@@ -5709,12 +5717,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B57" s="7" t="s">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>680</v>
+      </c>
+      <c r="C57" t="s">
         <v>600</v>
-      </c>
-      <c r="C57" t="s">
-        <v>677</v>
       </c>
       <c r="D57" t="s">
         <v>541</v>
@@ -5723,12 +5731,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B58" s="7" t="s">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>616</v>
+      </c>
+      <c r="C58" t="s">
         <v>601</v>
-      </c>
-      <c r="C58" t="s">
-        <v>678</v>
       </c>
       <c r="D58" t="s">
         <v>542</v>
@@ -5737,12 +5745,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B59" s="7" t="s">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>628</v>
+      </c>
+      <c r="C59" t="s">
         <v>602</v>
-      </c>
-      <c r="C59" t="s">
-        <v>679</v>
       </c>
       <c r="D59" t="s">
         <v>110</v>
@@ -5751,12 +5759,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B60" s="7" t="s">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C60" t="s">
         <v>603</v>
-      </c>
-      <c r="C60" t="s">
-        <v>680</v>
       </c>
       <c r="D60" t="s">
         <v>144</v>
@@ -5765,12 +5773,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B61" s="7" t="s">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>681</v>
+      </c>
+      <c r="C61" t="s">
         <v>604</v>
-      </c>
-      <c r="C61" t="s">
-        <v>681</v>
       </c>
       <c r="D61" t="s">
         <v>543</v>
@@ -5779,12 +5787,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B62" s="7" t="s">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>682</v>
+      </c>
+      <c r="C62" t="s">
         <v>605</v>
-      </c>
-      <c r="C62" t="s">
-        <v>682</v>
       </c>
       <c r="D62" t="s">
         <v>544</v>
@@ -5799,7 +5807,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5807,79 +5815,79 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="7" width="20.5" customWidth="1"/>
-    <col min="8" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>473</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>475</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>476</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>477</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>-1000</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>1000</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>485</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>488</v>
       </c>
     </row>

</xml_diff>